<commit_message>
tüm validasyonlar sağlanmadan işleme devam etmiyor
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/validationTest.xlsx
+++ b/WebApplication1/Forms/validationTest.xlsx
@@ -57,14 +57,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -351,17 +345,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="2"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
customFormattedCellTables listesi backendden gönderiliyor
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/validationTest.xlsx
+++ b/WebApplication1/Forms/validationTest.xlsx
@@ -28,6 +28,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[Red][&lt;50]0;[Red][&gt;100]0;0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -59,7 +62,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -345,7 +348,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
excelin backende post edilmesi yöntemi değiştirildi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/validationTest.xlsx
+++ b/WebApplication1/Forms/validationTest.xlsx
@@ -29,7 +29,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[Red][=50]0;[Red][=100]0;0"/>
+    <numFmt numFmtId="164" formatCode="[Red][=50]0;[Red][=100]0;0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -65,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -351,7 +351,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,9 +370,13 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="A1:B2">
+  <dataValidations count="2">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="A1:A2 B2">
       <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>0</formula1>
+      <formula2>120</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>